<commit_message>
added planned finish dates
</commit_message>
<xml_diff>
--- a/project time table.xlsx
+++ b/project time table.xlsx
@@ -179,11 +179,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -205,12 +206,20 @@
       <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="22"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -359,11 +368,11 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -375,7 +384,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -476,24 +485,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="D10:M81"/>
+  <dimension ref="D10:P81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P32" activeCellId="0" sqref="P32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N24" activeCellId="0" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="71.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.65"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.64"/>
   </cols>
   <sheetData>
     <row r="10" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -532,11 +537,16 @@
         <v>9</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
+      <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="9" t="s">
@@ -545,12 +555,19 @@
       <c r="E12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="8"/>
+      <c r="F12" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="9" t="s">
@@ -559,12 +576,19 @@
       <c r="E13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="8"/>
+      <c r="F13" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="9" t="s">
@@ -573,12 +597,19 @@
       <c r="E14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="8"/>
+      <c r="F14" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="9" t="s">
@@ -587,12 +618,19 @@
       <c r="E15" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
+      <c r="F15" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="9" t="s">
@@ -601,12 +639,19 @@
       <c r="E16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+      <c r="F16" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="5" t="s">
@@ -616,11 +661,16 @@
         <v>20</v>
       </c>
       <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="9" t="s">
@@ -630,11 +680,18 @@
         <v>17</v>
       </c>
       <c r="F18" s="7"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="8"/>
+      <c r="G18" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="9" t="s">
@@ -644,11 +701,18 @@
         <v>23</v>
       </c>
       <c r="F19" s="7"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="8"/>
+      <c r="G19" s="11" t="n">
+        <v>17</v>
+      </c>
+      <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="9" t="s">
@@ -658,11 +722,18 @@
         <v>15</v>
       </c>
       <c r="F20" s="7"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="8"/>
+      <c r="G20" s="11" t="n">
+        <v>19</v>
+      </c>
+      <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="9" t="s">
@@ -672,11 +743,18 @@
         <v>26</v>
       </c>
       <c r="F21" s="7"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="8"/>
+      <c r="G21" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="9" t="s">
@@ -686,11 +764,18 @@
         <v>28</v>
       </c>
       <c r="F22" s="7"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="8"/>
+      <c r="G22" s="11" t="n">
+        <v>30</v>
+      </c>
+      <c r="H22" s="7"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="9" t="s">
@@ -700,11 +785,18 @@
         <v>30</v>
       </c>
       <c r="F23" s="7"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="8"/>
+      <c r="G23" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="9" t="s">
@@ -714,11 +806,18 @@
         <v>17</v>
       </c>
       <c r="F24" s="7"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="8"/>
+      <c r="G24" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="9" t="s">
@@ -728,11 +827,18 @@
         <v>17</v>
       </c>
       <c r="F25" s="7"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
+      <c r="G25" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="5" t="s">
@@ -743,10 +849,15 @@
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D27" s="9" t="s">
@@ -757,10 +868,17 @@
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="8"/>
+      <c r="H27" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="9" t="s">
@@ -771,10 +889,17 @@
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="8"/>
+      <c r="H28" s="11" t="n">
+        <v>16</v>
+      </c>
+      <c r="I28" s="7"/>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
     </row>
     <row r="29" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D29" s="9" t="s">
@@ -785,10 +910,17 @@
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="8"/>
+      <c r="H29" s="11" t="n">
+        <v>21</v>
+      </c>
+      <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
     </row>
     <row r="30" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="9" t="s">
@@ -799,10 +931,17 @@
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="8"/>
+      <c r="H30" s="11" t="n">
+        <v>28</v>
+      </c>
+      <c r="I30" s="7"/>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D31" s="9" t="s">
@@ -813,10 +952,17 @@
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="8"/>
+      <c r="H31" s="11" t="n">
+        <v>29</v>
+      </c>
+      <c r="I31" s="7"/>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="5" t="s">
@@ -831,6 +977,11 @@
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="9" t="s">
@@ -842,9 +993,16 @@
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="8"/>
+      <c r="I33" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="J33" s="7"/>
       <c r="K33" s="7"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D34" s="9" t="s">
@@ -856,9 +1014,16 @@
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="8"/>
+      <c r="I34" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="J34" s="7"/>
       <c r="K34" s="7"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D35" s="9" t="s">
@@ -870,9 +1035,16 @@
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="8"/>
+      <c r="I35" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="J35" s="7"/>
       <c r="K35" s="7"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D36" s="9" t="s">
@@ -884,9 +1056,16 @@
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="8"/>
+      <c r="I36" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="J36" s="7"/>
       <c r="K36" s="7"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D37" s="9" t="s">
@@ -898,9 +1077,16 @@
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="8"/>
+      <c r="I37" s="11" t="n">
+        <v>14</v>
+      </c>
+      <c r="J37" s="7"/>
       <c r="K37" s="7"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D38" s="12" t="s">
@@ -915,6 +1101,11 @@
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
     </row>
     <row r="39" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D39" s="9" t="s">
@@ -927,8 +1118,15 @@
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
-      <c r="J39" s="11"/>
+      <c r="J39" s="11" t="n">
+        <v>18</v>
+      </c>
       <c r="K39" s="11"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D40" s="14" t="s">
@@ -941,8 +1139,15 @@
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
-      <c r="J40" s="11"/>
+      <c r="J40" s="11" t="n">
+        <v>19</v>
+      </c>
       <c r="K40" s="11"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E41" s="10"/>

</xml_diff>